<commit_message>
Build 2024ver FC pinout, change MCU to STM32H743ZIT6
</commit_message>
<xml_diff>
--- a/Published/APP_6DOF/rocket_properties/Launch1 mass properties.xlsx
+++ b/Published/APP_6DOF/rocket_properties/Launch1 mass properties.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\AvionicsDev\Published\APP_6DOF\rocket_properties\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D72FD-417E-4CF5-B6B4-87C23A06724A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -64,22 +73,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -88,7 +107,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -104,40 +123,45 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -148,11 +172,17 @@
     <xdr:ext cx="1362075" cy="3505200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
+        <xdr:cNvPr id="2" name="image1.png" title="圖片">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -170,7 +200,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -360,24 +390,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.63"/>
-    <col customWidth="1" min="3" max="3" width="13.25"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -398,87 +433,239 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>15.58</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>-0.912</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>-0.91200000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
-        <v>-543.08</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>-543.08000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5">
-        <v>4.446</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4.4459999999999997</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5">
-        <v>1176913.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1176913</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5">
-        <v>-383.374</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>-383.37400000000002</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5">
-        <v>-46.754</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>-46.753999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5">
         <v>138861.1</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>-6918.36</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5">
-        <v>1160217.0</v>
+        <v>1160217</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>